<commit_message>
Reorder chocolate attribute levels; DS-2197
</commit_message>
<xml_diff>
--- a/inst/extdata/chocolate_attributes.xlsx
+++ b/inst/extdata/chocolate_attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathew\Documents\Features\ChoiceModelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65BE7B4-5466-4BB9-BF7D-77DC752FC2A4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F539DC56-77D8-4A23-BD02-604F455D873F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Brand</t>
   </si>
@@ -103,25 +103,19 @@
     <t>No</t>
   </si>
   <si>
+    <t>Lindt</t>
+  </si>
+  <si>
+    <t>$2.49</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Lindt</t>
-  </si>
-  <si>
-    <t>$2.49</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>Belgian (Single origin Venezuelan Criollo beans)</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t/>
@@ -443,7 +437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -481,7 +477,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
@@ -490,10 +486,10 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -513,10 +509,10 @@
         <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -527,7 +523,7 @@
         <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>24</v>
@@ -536,33 +532,27 @@
         <v>25</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename attribute level; DS-2197
</commit_message>
<xml_diff>
--- a/inst/extdata/chocolate_attributes.xlsx
+++ b/inst/extdata/chocolate_attributes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathew\Documents\Features\ChoiceModelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F539DC56-77D8-4A23-BD02-604F455D873F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875236DC-E39F-4ECB-AEAE-5C68A558134A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,10 +115,10 @@
     <t/>
   </si>
   <si>
-    <t>Belgian (Single origin Venezuelan Criollo beans)</t>
-  </si>
-  <si>
     <t/>
+  </si>
+  <si>
+    <t>Belgium (Single origin Venezuelan Criollo beans)</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,10 +549,10 @@
         <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>